<commit_message>
Incluido tarefa de crescimento automatico do banco
git-svn-id: https://portal.cc.com.br:8084/svn/projetos@1879 236fd033-a1ae-4692-b96d-e3c3cfb81559
</commit_message>
<xml_diff>
--- a/Procedimentos/Plano de alteração de IP e instalação SQL Server.xlsx
+++ b/Procedimentos/Plano de alteração de IP e instalação SQL Server.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Sequência</t>
   </si>
@@ -104,12 +104,18 @@
   </si>
   <si>
     <t>Carregar o script para a criação dos JOB´s (arq. já esta na maq. Compreing)</t>
+  </si>
+  <si>
+    <t>Configurar a taxa de crescimento automática dos bancos para 100MB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="h:mm"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -206,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -228,13 +234,14 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="25" formatCode="h:mm"/>
+      <numFmt numFmtId="164" formatCode="h:mm"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -258,8 +265,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:D20" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A2:D20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:D21" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="A2:D21"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Sequência"/>
     <tableColumn id="2" name="Tarefa"/>
@@ -555,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -778,27 +785,27 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="10">
-        <v>6.9444444444444441E-3</v>
+      <c r="D16" s="13">
+        <v>3.472222222222222E-3</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>10</v>
+      <c r="B17" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D17" s="10">
-        <v>3.472222222222222E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -806,42 +813,56 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D18" s="10">
-        <v>6.9444444444444441E-3</v>
+        <v>3.472222222222222E-3</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="10">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="B20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D20" s="10">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="11" t="s">
+    <row r="21" spans="1:4">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="12">
-        <f>SUM(D3:D19)</f>
-        <v>0.23958333333333331</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="B21" s="1"/>
+      <c r="D21" s="12">
+        <f>SUM(D3:D20)</f>
+        <v>0.24305555555555552</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="B22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
atualização com o resultado das atividades
git-svn-id: https://portal.cc.com.br:8084/svn/projetos@1893 236fd033-a1ae-4692-b96d-e3c3cfb81559
</commit_message>
<xml_diff>
--- a/Procedimentos/Plano de alteração de IP e instalação SQL Server.xlsx
+++ b/Procedimentos/Plano de alteração de IP e instalação SQL Server.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
   <si>
     <t>Sequência</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Plano de alteração de IP´s das máquinas do Datacenter de Campinas e Instalação de SQLServer 2005 32bits</t>
-  </si>
-  <si>
-    <t>Carregar o script para a criação dos JOB´s (arq. já esta na maq. Compreing)</t>
   </si>
   <si>
     <t>07:45h</t>
@@ -173,12 +170,52 @@
   </si>
   <si>
     <t>Efetuar testes de acesso externo com novo IP e com novo SqlServer 2005 sem tirar a página de manutenção do ar e simular uma compra com cartão inválido; usar url da tarefa 1.</t>
+  </si>
+  <si>
+    <t>hora realizada - inicio</t>
+  </si>
+  <si>
+    <t>hora realizada - final</t>
+  </si>
+  <si>
+    <t>Nâo foi passado os IP´s antecipadamente como combinado para alteração na locaweb</t>
+  </si>
+  <si>
+    <t>08:00h</t>
+  </si>
+  <si>
+    <t>08:05h</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Não OK; atividade cancelada</t>
+  </si>
+  <si>
+    <t>Não OK; atraso na definição dos ips e configuração do Firewall junto a MIX; atividade cancelada devido a falta de tempo para viabilizar a execução</t>
+  </si>
+  <si>
+    <t>Carregar o script para a criação dos JOB´s e criação dos usuários (arq. já esta na maq. Compreing)</t>
+  </si>
+  <si>
+    <t>Instalação do driver do cliente do sqlserver 2008 
+http://go.microsoft.com/fwlink/?LinkId=163712</t>
+  </si>
+  <si>
+    <t>Não ocorreu a alteração dos IP´s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="h:mm"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -210,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +263,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -272,19 +315,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="h:mm"/>
     </dxf>
@@ -310,18 +382,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:F23" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A2:F23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:I25" totalsRowShown="0" tableBorderDxfId="4">
+  <autoFilter ref="A2:I25">
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
+    <filterColumn colId="6"/>
+    <filterColumn colId="7"/>
+    <filterColumn colId="8"/>
   </autoFilter>
-  <tableColumns count="6">
+  <tableColumns count="9">
     <tableColumn id="1" name="Sequência"/>
     <tableColumn id="2" name="Tarefa"/>
     <tableColumn id="3" name="Responsável"/>
-    <tableColumn id="4" name="Tempo Estimado_x000a_(minutos)" dataDxfId="0"/>
+    <tableColumn id="4" name="Tempo Estimado_x000a_(minutos)" dataDxfId="3"/>
     <tableColumn id="5" name="Previsão de Início"/>
     <tableColumn id="6" name="Previsão de Término"/>
+    <tableColumn id="7" name="hora realizada - inicio" dataDxfId="2"/>
+    <tableColumn id="8" name="hora realizada - final" dataDxfId="1"/>
+    <tableColumn id="9" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -612,33 +690,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" customWidth="1"/>
+    <col min="2" max="2" width="66" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="53.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:9" ht="18.75">
+      <c r="A1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:6" ht="30">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+    </row>
+    <row r="2" spans="1:9" ht="45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -652,18 +735,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>3</v>
@@ -672,13 +764,22 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="12">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="H3" s="12">
+        <v>0.32361111111111113</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -692,13 +793,22 @@
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>21</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0.33124999999999999</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0.33194444444444443</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -712,357 +822,513 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="42.75" customHeight="1">
-      <c r="A6" s="2">
+        <v>20</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="15">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="78.75" customHeight="1">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D7" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.5" customHeight="1">
-      <c r="A7" s="2">
+      <c r="E7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.5" customHeight="1">
+      <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D8" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30">
-      <c r="A8" s="2">
+      <c r="E8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30">
+      <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="D8" s="7">
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D9" s="7">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="7">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>38</v>
+      </c>
+      <c r="G10" s="12">
+        <v>0.3840277777777778</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0.39097222222222222</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30">
       <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>24</v>
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="12">
+        <v>0.39097222222222222</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0.41111111111111115</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="7">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="2">
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0.41111111111111115</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0.41250000000000003</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="7">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45">
-      <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="7">
-        <v>2.0833333333333332E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>40</v>
+      </c>
+      <c r="G13" s="12">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45">
       <c r="A14" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D14" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="12">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
         <v>43</v>
       </c>
-      <c r="F14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="2">
+      <c r="G15" s="12">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="H15" s="12">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30">
+      <c r="A16" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D15" s="7">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30">
-      <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="D16" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30">
+      <c r="G16" s="12">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45">
       <c r="A17" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D17" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30">
+      <c r="A18" s="2"/>
+      <c r="B18" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="18">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="H18" s="18">
+        <v>0.49374999999999997</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30">
+      <c r="A19" s="2">
+        <v>15</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="7">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" t="s">
         <v>32</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G19" s="12">
+        <v>0.49374999999999997</v>
+      </c>
+      <c r="H19" s="12">
+        <v>0.49513888888888885</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="2">
+        <v>16</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="7">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="2">
+        <v>17</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="7">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2">
+      <c r="G21" s="12">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="H21" s="12">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="7">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="2">
-        <v>17</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="7">
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="E19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="13">
-        <f>SUBTOTAL(109,D3:D19)</f>
-        <v>0.18402777777777779</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="2">
+      <c r="D22" s="11">
+        <f>SUBTOTAL(109,D3:D21)</f>
+        <v>0.18750000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="2">
         <v>18</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="7">
-        <v>6.9444444444444441E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30">
-      <c r="A22" s="2">
-        <v>19</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="7">
-        <v>3.472222222222222E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="2">
-        <v>20</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>29</v>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="7">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30">
+      <c r="A24" s="2">
+        <v>19</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="7">
         <v>3.472222222222222E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="2"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="B25" s="1"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="2">
+        <v>20</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="7">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="2"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="B27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>